<commit_message>
Added content type control
Added content type control from Import File
Updated Output
</commit_message>
<xml_diff>
--- a/Import-Format.xlsx
+++ b/Import-Format.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:dbsheet="http://web.wps.cn/et/2021/dbsheet">
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="27945" windowHeight="12180"/>
+    <workbookView windowWidth="24750" windowHeight="10400"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="17">
   <si>
     <t>Title</t>
   </si>
@@ -42,30 +42,40 @@
     <t>Excerpt</t>
   </si>
   <si>
-    <t>Card Image
-(format: https://)</t>
-  </si>
-  <si>
     <t>Featured Image
 (format: https://)</t>
   </si>
   <si>
-    <t>Intro Text</t>
-  </si>
-  <si>
     <t>Editor</t>
   </si>
   <si>
-    <t>Orange Text</t>
-  </si>
-  <si>
-    <t>Source of information</t>
-  </si>
-  <si>
     <t>Tags</t>
   </si>
   <si>
-    <t>News/Inspiration</t>
+    <r>
+      <t xml:space="preserve">Content Type ID
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(contentTypeId)</t>
+    </r>
+  </si>
+  <si>
+    <t>Post Title</t>
+  </si>
+  <si>
+    <t>post-title</t>
+  </si>
+  <si>
+    <t>Lorem Ipsum</t>
   </si>
   <si>
     <t>https://picsum.photos/536/354</t>
@@ -75,6 +85,15 @@
   </si>
   <si>
     <t>test 11,test 22</t>
+  </si>
+  <si>
+    <t>news</t>
+  </si>
+  <si>
+    <t>Demo Title</t>
+  </si>
+  <si>
+    <t>demo-title</t>
   </si>
 </sst>
 </file>
@@ -88,7 +107,7 @@
     <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="180" formatCode="dd/mm/yyyy\ hh:mm"/>
   </numFmts>
-  <fonts count="21">
+  <fonts count="22">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -246,6 +265,14 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -705,8 +732,11 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1">
@@ -715,10 +745,16 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="6">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="6" applyFill="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -729,7 +765,7 @@
     <cellStyle name="Percent" xfId="3" builtinId="5"/>
     <cellStyle name="Comma [0]" xfId="4" builtinId="6"/>
     <cellStyle name="Currency [0]" xfId="5" builtinId="7"/>
-    <cellStyle name="Hyperlink" xfId="6" builtinId="8"/>
+    <cellStyle name="Link" xfId="6" builtinId="8"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9"/>
     <cellStyle name="Note" xfId="8" builtinId="10"/>
     <cellStyle name="Warning Text" xfId="9" builtinId="11"/>
@@ -1254,100 +1290,103 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:L2"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="1"/>
+  <sheetFormatPr defaultColWidth="9.14545454545454" defaultRowHeight="14.5" outlineLevelRow="2" outlineLevelCol="7"/>
   <cols>
-    <col min="1" max="1" width="6.71428571428571" customWidth="1"/>
-    <col min="3" max="5" width="16.7142857142857"/>
-    <col min="6" max="6" width="31.5714285714286" customWidth="1"/>
-    <col min="7" max="7" width="16.7142857142857"/>
-    <col min="8" max="8" width="29.0571428571429" customWidth="1"/>
-    <col min="9" max="10" width="25.1428571428571" customWidth="1"/>
-    <col min="12" max="12" width="17.8571428571429" customWidth="1"/>
+    <col min="1" max="1" width="6.71818181818182" customWidth="1"/>
+    <col min="3" max="4" width="16.7181818181818"/>
+    <col min="5" max="5" width="31.5727272727273" customWidth="1"/>
+    <col min="6" max="6" width="29.0545454545455" customWidth="1"/>
+    <col min="8" max="8" width="17.8545454545455" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="45" spans="1:12">
-      <c r="A1" s="1" t="s">
+    <row r="1" ht="43.5" spans="1:8">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+    </row>
+    <row r="2" s="1" customFormat="1" spans="1:8">
+      <c r="A2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="B2" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="C2" s="6">
+        <v>45916.5105324074</v>
+      </c>
+      <c r="D2" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="E2" s="7" t="s">
         <v>11</v>
       </c>
+      <c r="F2" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="2" spans="1:11">
-      <c r="A2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="3">
-        <v>45638.5938657407</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" s="4" t="s">
+    <row r="3" s="1" customFormat="1" spans="1:8">
+      <c r="A3" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="6">
+        <v>45916.5105324074</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H2" s="1" t="s">
+      <c r="G3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="I2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K2" t="s">
+      <c r="H3" s="1" t="s">
         <v>14</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1" display="https://picsum.photos/536/354"/>
     <hyperlink ref="E2" r:id="rId1" display="https://picsum.photos/536/354"/>
+    <hyperlink ref="E3" r:id="rId1" display="https://picsum.photos/536/354"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>